<commit_message>
data cleaning summaries for 2019
</commit_message>
<xml_diff>
--- a/2019/cleaning_summary/destination_simple.xlsx
+++ b/2019/cleaning_summary/destination_simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-studies\2017\summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SChildress\Documents\GitHub\travel-studies\2019\cleaning_summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D3F73-8CC1-4E99-9EFE-79BD5329918D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB64B1DE-3BF3-48AF-ADAF-D90A0D1133DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{5730C50B-1828-491D-A1B6-3C75870F173B}"/>
+    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{5730C50B-1828-491D-A1B6-3C75870F173B}"/>
   </bookViews>
   <sheets>
     <sheet name="destination_simple" sheetId="1" r:id="rId1"/>
@@ -104,13 +104,13 @@
     <t>Work</t>
   </si>
   <si>
+    <t>Recreation/Eat Meal</t>
+  </si>
+  <si>
+    <t>Errands and Shopping</t>
+  </si>
+  <si>
     <t>Destination purpose</t>
-  </si>
-  <si>
-    <t>Recreation/Eat Meal</t>
-  </si>
-  <si>
-    <t>Errands and Shopping</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -573,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +581,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,7 +613,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>